<commit_message>
Card details, Font adjustment, grading number added, Drop Down navigation works, Spreadsheet empty cells crash issue, Started multiple cells selection
</commit_message>
<xml_diff>
--- a/GradesGuru/Data/Centering.xlsx
+++ b/GradesGuru/Data/Centering.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>Grade</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Ex-NM+</t>
+  </si>
+  <si>
+    <t>10/10</t>
   </si>
   <si>
     <t>Ex/NM</t>
@@ -217,19 +220,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -239,42 +248,66 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -286,25 +319,65 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -313,51 +386,78 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,6 +476,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff111111"/>
     </indexedColors>
@@ -576,12 +677,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -614,10 +715,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -865,12 +966,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1185,10 +1286,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1442,7 +1543,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1451,7 +1552,8 @@
     <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.1719" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1467,214 +1569,235 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="5">
         <v>6</v>
       </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="4">
+      <c r="D7" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="D8" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>3</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D9" t="s" s="4">
+      <c r="D9" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D10" t="s" s="4">
+      <c r="D10" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>1.5</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D11" t="s" s="4">
+      <c r="D11" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="D12" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1690,17 +1813,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.67188" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="31.3516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.67188" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="31.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1713,217 +1837,238 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="D1" t="s" s="10">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" t="s" s="11">
         <v>23</v>
       </c>
-      <c r="D2" t="s" s="9">
+      <c r="D2" t="s" s="12">
         <v>24</v>
       </c>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>9.5</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="11">
         <v>25</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" t="s" s="12">
         <v>24</v>
       </c>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="D4" t="s" s="14">
         <v>27</v>
       </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" t="s" s="5">
         <v>29</v>
       </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" t="s" s="5">
         <v>31</v>
       </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="D7" t="s" s="4">
+      <c r="D7" t="s" s="5">
         <v>33</v>
       </c>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" t="s" s="5">
         <v>34</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="D8" t="s" s="5">
         <v>33</v>
       </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>4</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" t="s" s="5">
         <v>35</v>
       </c>
-      <c r="D9" t="s" s="4">
+      <c r="D9" t="s" s="5">
         <v>36</v>
       </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="D10" t="s" s="4">
+      <c r="D10" t="s" s="5">
         <v>36</v>
       </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>2</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="D11" t="s" s="4">
+      <c r="D11" t="s" s="5">
         <v>39</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" t="s" s="5">
         <v>40</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="D12" t="s" s="5">
         <v>40</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1939,18 +2084,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="14.5" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="14.5" style="11" customWidth="1"/>
+    <col min="1" max="5" width="14.5" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="12">
+      <c r="A1" t="s" s="16">
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
@@ -1959,232 +2104,284 @@
       <c r="C1" t="s" s="2">
         <v>41</v>
       </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="C2" t="s" s="13">
+      <c r="C2" t="s" s="19">
         <v>42</v>
       </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" ht="14.6" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="11">
         <v>43</v>
       </c>
-      <c r="C3" t="s" s="14">
+      <c r="C3" t="s" s="21">
         <v>44</v>
       </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" ht="14.6" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>9.5</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="11">
         <v>45</v>
       </c>
-      <c r="C4" t="s" s="14">
+      <c r="C4" t="s" s="21">
         <v>44</v>
       </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" t="s" s="14">
         <v>5</v>
       </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <f>A5-0.5</f>
         <v>8.5</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="5">
         <v>46</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" t="s" s="5">
         <v>8</v>
       </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <f>A6-0.5</f>
         <v>8</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" t="s" s="5">
         <v>8</v>
       </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <f>A7-0.5</f>
         <v>7.5</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="5">
         <v>47</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" t="s" s="5">
         <v>11</v>
       </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <f>A8-0.5</f>
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" t="s" s="5">
         <v>11</v>
       </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <f>A9-0.5</f>
         <v>6.5</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" t="s" s="5">
         <v>48</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <f>A10-0.5</f>
         <v>6</v>
       </c>
-      <c r="B11" t="s" s="4">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s" s="4">
+      <c r="B11" t="s" s="5">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s" s="5">
         <v>6</v>
       </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <f>A11-0.5</f>
         <v>5.5</v>
       </c>
-      <c r="B12" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="C12" s="5"/>
+      <c r="B12" t="s" s="5">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <f>A12-0.5</f>
         <v>5</v>
       </c>
-      <c r="B13" t="s" s="4">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s" s="4">
+      <c r="B13" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s" s="5">
         <v>14</v>
       </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <f>A13-0.5</f>
         <v>4.5</v>
       </c>
-      <c r="B14" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="C14" s="5"/>
+      <c r="B14" t="s" s="5">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <f>A14-0.5</f>
         <v>4</v>
       </c>
-      <c r="B15" t="s" s="4">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s" s="4">
+      <c r="B15" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s" s="5">
         <v>16</v>
       </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <f>A15-0.5</f>
         <v>3.5</v>
       </c>
-      <c r="B16" t="s" s="4">
-        <v>54</v>
-      </c>
-      <c r="C16" s="5"/>
+      <c r="B16" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <f>A16-0.5</f>
         <v>3</v>
       </c>
-      <c r="B17" t="s" s="4">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s" s="4">
+      <c r="B17" t="s" s="5">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <f>A17-0.5</f>
         <v>2.5</v>
       </c>
-      <c r="B18" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s" s="4">
+      <c r="B18" t="s" s="5">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <f>A18-0.5</f>
         <v>2</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="B19" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="C19" t="s" s="4">
+      <c r="C19" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <f>A19-0.5</f>
         <v>1.5</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" t="s" s="5">
         <v>9</v>
       </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <f>A20-0.5</f>
         <v>1</v>
       </c>
-      <c r="B21" t="s" s="4">
+      <c r="B21" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>